<commit_message>
Bug fixes and fresh data
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/countries/Algeria.xlsx
+++ b/a-place-for-salvador-allende/countries/Algeria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3147221CDA41D307846E3F816C7844056243FAA1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC0A785-7D1B-45EA-BD7A-B95484EA6712}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_3147221CDA41D307846E3F816C7844056243FAA1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63520AB-94A2-4866-8816-A18542AB5FB0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -97,9 +97,6 @@
     <t>abacq_reference</t>
   </si>
   <si>
-    <t>ساحة سلفادور ألندي</t>
-  </si>
-  <si>
     <t>park</t>
   </si>
   <si>
@@ -125,6 +122,15 @@
   </si>
   <si>
     <t>http://www.abacq.org/calle/index.php?2007/03/11/51-argel-argelia</t>
+  </si>
+  <si>
+    <t>ساحة سلفادور ألندي 	Place Salvador Allende</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/9QP1kuoswBG4RZ1s9</t>
+  </si>
+  <si>
+    <t>abacq date posted</t>
   </si>
 </sst>
 </file>
@@ -542,7 +548,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,32 +631,32 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>103</v>
+      </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
       </c>
       <c r="L2">
         <v>36.753338499999998</v>
@@ -667,20 +673,27 @@
       <c r="P2">
         <v>11</v>
       </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
       <c r="V2">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="W2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="Y2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="X2" r:id="rId3" xr:uid="{9E4D8E47-058D-4EE3-8E9D-675FBA2D214A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>